<commit_message>
Updated documentation for release
</commit_message>
<xml_diff>
--- a/Other Files/parts_list.xlsx
+++ b/Other Files/parts_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nils\Documents\Saxion\projects\CHARISMA\spot_backpack_solidworks\Other Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF14D3D7-1D81-40A6-B4C9-D24C69FC7F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598AB1AA-8DA7-48F5-A9D9-670DFA731AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-61548" yWindow="1932" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="144">
   <si>
     <t>Amount</t>
   </si>
@@ -294,18 +294,6 @@
     <t>2491569</t>
   </si>
   <si>
-    <t>Stuks</t>
-  </si>
-  <si>
-    <t>Neutrik NAHDMI-W HDMI-connector Flensbus, contacten recht Aantal polen: 19 Zilver 1 stuk(s)</t>
-  </si>
-  <si>
-    <t>https://www.conrad.nl/nl/p/neutrik-nahdmi-w-hdmi-connector-flensbus-contacten-recht-aantal-polen-19-zilver-1-stuk-s-733854.html</t>
-  </si>
-  <si>
-    <t>733854 - 8J</t>
-  </si>
-  <si>
     <t>Price may differ depending on how many parts you order. This quote of this order included some backup parts as well parts specific to the CHARISMA project, which may not be needed for your project.</t>
   </si>
   <si>
@@ -315,9 +303,6 @@
     <t>https://www.robotlab.com/store/-ports</t>
   </si>
   <si>
-    <t>Not clear if price with or without VAT; price is converted from dollars to euros</t>
-  </si>
-  <si>
     <t>WIFI antenna (Female RP-SMA)</t>
   </si>
   <si>
@@ -478,6 +463,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>This cable is specific to the PC we used (VECOW SPC7000) which had displayports. Only order this if your PC also uses displayports instead of HDMI, e.g. https://nl.rs-online.com/web/p/hdmi-cables/1765697?gb=s</t>
+  </si>
+  <si>
+    <t>NOTE: This site is out of date! Probably best to contact Boston Dynamics directly and ask for a quote / vendor!</t>
   </si>
 </sst>
 </file>
@@ -663,7 +654,7 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -687,6 +678,8 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Accent2" xfId="5" builtinId="35"/>
@@ -995,24 +988,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" customWidth="1"/>
-    <col min="9" max="9" width="24.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="74.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" customWidth="1"/>
+    <col min="5" max="5" width="16.26953125" customWidth="1"/>
+    <col min="6" max="6" width="14.26953125" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" customWidth="1"/>
+    <col min="8" max="8" width="16.81640625" customWidth="1"/>
+    <col min="9" max="9" width="24.54296875" customWidth="1"/>
+    <col min="10" max="10" width="12.81640625" customWidth="1"/>
+    <col min="11" max="11" width="74.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1044,7 +1037,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>42</v>
       </c>
@@ -1058,7 +1051,7 @@
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1094,7 +1087,7 @@
       </c>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1111,7 +1104,7 @@
         <v>16</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:F13" si="0">IF(ISNUMBER(G5), G5 * (0.79), "")</f>
+        <f t="shared" ref="F5:F12" si="0">IF(ISNUMBER(G5), G5 * (0.79), "")</f>
         <v>11.8421</v>
       </c>
       <c r="G5">
@@ -1126,7 +1119,7 @@
         <v>29.98</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1158,7 +1151,7 @@
         <v>77.989999999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1190,7 +1183,7 @@
         <v>45.99</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1222,7 +1215,7 @@
         <v>45.99</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1254,7 +1247,7 @@
         <v>44.99</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1286,7 +1279,7 @@
         <v>59.96</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1322,7 +1315,7 @@
       </c>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1358,39 +1351,7 @@
       </c>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" t="s">
-        <v>86</v>
-      </c>
-      <c r="D13" t="s">
-        <v>87</v>
-      </c>
-      <c r="E13" t="s">
-        <v>88</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>14.2121</v>
-      </c>
-      <c r="G13">
-        <v>17.989999999999998</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="1"/>
-        <v>14.2121</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="2"/>
-        <v>17.989999999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G14" t="str">
         <f t="shared" ref="G14:G16" si="3">IF(ISNUMBER(F14), F14 * (1 + 0.21), "")</f>
         <v/>
@@ -1404,7 +1365,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G15" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -1418,7 +1379,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
         <v>43</v>
       </c>
@@ -1441,7 +1402,7 @@
       </c>
       <c r="J16" s="15"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1470,10 +1431,10 @@
         <v>244.29900000000001</v>
       </c>
       <c r="J17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1496,7 +1457,7 @@
         <v>7.5625</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1519,7 +1480,7 @@
         <v>11.616</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G20" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1533,7 +1494,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
         <v>49</v>
       </c>
@@ -1556,7 +1517,7 @@
       </c>
       <c r="J21" s="15"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1591,7 +1552,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1623,7 +1584,7 @@
         <v>76.556700000000006</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1646,7 +1607,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1654,10 +1615,10 @@
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D25" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E25" t="s">
         <v>46</v>
@@ -1677,11 +1638,11 @@
         <f t="shared" si="2"/>
         <v>1429.2641000000001</v>
       </c>
-      <c r="J25" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J25" s="18" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1689,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D26" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E26">
         <v>1084927</v>
@@ -1713,7 +1674,7 @@
         <v>25.38</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1721,13 +1682,13 @@
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>95</v>
-      </c>
-      <c r="D27" t="s">
-        <v>98</v>
+        <v>90</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>93</v>
       </c>
       <c r="E27" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F27">
         <f t="shared" ref="F27:F30" si="5">IF(ISNUMBER(G27), G27 * (0.79), "")</f>
@@ -1745,7 +1706,7 @@
         <v>7.98</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1753,10 +1714,10 @@
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D28" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E28">
         <v>401013476</v>
@@ -1777,7 +1738,7 @@
         <v>6.44</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1785,13 +1746,13 @@
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D29" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E29" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F29">
         <f t="shared" si="5"/>
@@ -1809,7 +1770,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>4</v>
       </c>
@@ -1817,13 +1778,13 @@
         <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D30" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E30" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F30">
         <f t="shared" si="5"/>
@@ -1841,7 +1802,7 @@
         <v>31.16</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>10</v>
       </c>
@@ -1849,13 +1810,13 @@
         <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D31" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E31" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F31">
         <v>0.61</v>
@@ -1873,10 +1834,10 @@
         <v>7.3810000000000002</v>
       </c>
       <c r="J31" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G32" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1890,7 +1851,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G33" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1904,7 +1865,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="15" t="s">
         <v>57</v>
       </c>
@@ -1927,7 +1888,7 @@
       </c>
       <c r="J34" s="15"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>1</v>
       </c>
@@ -1962,7 +1923,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>3</v>
       </c>
@@ -1994,7 +1955,7 @@
         <v>26.549999999999997</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>1</v>
       </c>
@@ -2026,7 +1987,7 @@
         <v>57.72</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>1</v>
       </c>
@@ -2058,7 +2019,7 @@
         <v>20.07</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>1</v>
       </c>
@@ -2066,13 +2027,13 @@
         <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D39" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E39" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F39">
         <v>3.23</v>
@@ -2090,7 +2051,7 @@
         <v>3.9082999999999997</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>1</v>
       </c>
@@ -2098,13 +2059,13 @@
         <v>58</v>
       </c>
       <c r="C40" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D40" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E40" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F40">
         <f>IF(ISNUMBER(G40), G40* (0.79), "")</f>
@@ -2122,10 +2083,10 @@
         <v>34.5</v>
       </c>
       <c r="J40" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>1</v>
       </c>
@@ -2133,13 +2094,13 @@
         <v>58</v>
       </c>
       <c r="C41" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D41" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E41" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F41">
         <f t="shared" ref="F41:F47" si="7">IF(ISNUMBER(G41), G41* (0.79), "")</f>
@@ -2157,7 +2118,7 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>1</v>
       </c>
@@ -2165,13 +2126,13 @@
         <v>58</v>
       </c>
       <c r="C42" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D42" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E42" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F42">
         <f t="shared" si="7"/>
@@ -2189,7 +2150,7 @@
         <v>23.92</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>1</v>
       </c>
@@ -2197,13 +2158,13 @@
         <v>58</v>
       </c>
       <c r="C43" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D43" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E43" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F43">
         <f t="shared" si="7"/>
@@ -2221,7 +2182,7 @@
         <v>24.62</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>1</v>
       </c>
@@ -2229,13 +2190,13 @@
         <v>58</v>
       </c>
       <c r="C44" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D44" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E44" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F44">
         <f t="shared" si="7"/>
@@ -2253,7 +2214,7 @@
         <v>27.04</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>1</v>
       </c>
@@ -2261,13 +2222,13 @@
         <v>58</v>
       </c>
       <c r="C45" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D45" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E45" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F45">
         <f t="shared" si="7"/>
@@ -2285,7 +2246,7 @@
         <v>27.35</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>1</v>
       </c>
@@ -2293,13 +2254,13 @@
         <v>58</v>
       </c>
       <c r="C46" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D46" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E46" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F46">
         <f t="shared" si="7"/>
@@ -2317,7 +2278,7 @@
         <v>13.26</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>1</v>
       </c>
@@ -2325,13 +2286,13 @@
         <v>58</v>
       </c>
       <c r="C47" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D47" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E47" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F47">
         <f t="shared" si="7"/>
@@ -2349,7 +2310,7 @@
         <v>9.33</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G48" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2363,7 +2324,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G49" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2377,7 +2338,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G50" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2391,7 +2352,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="15" t="s">
         <v>72</v>
       </c>
@@ -2414,7 +2375,7 @@
       </c>
       <c r="J51" s="15"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>1</v>
       </c>
@@ -2446,7 +2407,7 @@
         <v>7.9134000000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>1</v>
       </c>
@@ -2478,7 +2439,7 @@
         <v>17.670000000000002</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>5</v>
       </c>
@@ -2510,7 +2471,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>1</v>
       </c>
@@ -2541,8 +2502,11 @@
         <f t="shared" si="2"/>
         <v>5.8200999999999992</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J55" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>1</v>
       </c>
@@ -2550,10 +2514,10 @@
         <v>10</v>
       </c>
       <c r="C56" t="s">
-        <v>100</v>
-      </c>
-      <c r="D56" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D56" s="17" t="s">
+        <v>96</v>
       </c>
       <c r="E56">
         <v>2920966</v>
@@ -2574,64 +2538,66 @@
         <v>3.4121999999999999</v>
       </c>
       <c r="J56" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="I57" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="I58" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="I59" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="I60" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="I61" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="I62" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G63" s="16" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="H63" s="16">
         <f>SUM(H3:H62)</f>
-        <v>2222.6815000000001</v>
+        <v>2208.4694</v>
       </c>
       <c r="I63" s="16">
         <f>SUM(I3:I62)</f>
-        <v>2730.5833000000002</v>
+        <v>2712.5933000000005</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D54" r:id="rId1" xr:uid="{954C0150-D23E-4514-8DB2-0ECB39BCA1E4}"/>
+    <hyperlink ref="D56" r:id="rId2" xr:uid="{6FA1ECF5-019A-4BF0-9AD1-0693C3D1AC81}"/>
+    <hyperlink ref="D27" r:id="rId3" xr:uid="{3806FCDE-1CF6-4692-AD6F-25D08A88B13B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2643,29 +2609,29 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="str">
         <f>IF(ISBLANK(SupplierTable[[#This Row],[Supplier]]),"", SupplierTable[[#This Row],[Supplier]] &amp; " (" &amp;ROUND(( SupplierTable[[#This Row],[Multiplier]]-1)*100, 0) &amp; "%)")</f>
         <v>TessaTronic (8%)</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C3" s="9">
         <v>1.08</v>
@@ -2674,25 +2640,25 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="str">
         <f>IF(ISBLANK(SupplierTable[[#This Row],[Supplier]]),"", SupplierTable[[#This Row],[Supplier]] &amp; " (" &amp;ROUND(( SupplierTable[[#This Row],[Multiplier]]-1)*100, 0) &amp; "%)")</f>
         <v>TessaTronic (15%)</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C4" s="13">
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="str">
         <f>IF(ISBLANK(SupplierTable[[#This Row],[Supplier]]),"", SupplierTable[[#This Row],[Supplier]] &amp; " (" &amp;ROUND(( SupplierTable[[#This Row],[Multiplier]]-1)*100, 0) &amp; "%)")</f>
         <v>TessaTronic (25%)</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C5" s="13">
         <v>1.25</v>

</xml_diff>